<commit_message>
Update CDP and DPR
Atualizado o CDP conforme execução do projeto e o DRP conforme o CDM-3.
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDP.xlsx
+++ b/Projeto/GPR/PG2016-1-CDP.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\GitHub\PSW\Projeto\GPR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Desktop\PSW\Projeto\GPR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
   <si>
     <t>ID da Atividade</t>
   </si>
@@ -617,44 +617,44 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1682,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1700,20 +1700,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2085,7 +2085,7 @@
         <v>8</v>
       </c>
       <c r="I13" s="7">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="J13" s="20" t="s">
         <v>58</v>
@@ -2177,7 +2177,9 @@
       <c r="I16" s="7">
         <v>300</v>
       </c>
-      <c r="J16" s="20"/>
+      <c r="J16" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
@@ -2205,9 +2207,11 @@
         <v>8</v>
       </c>
       <c r="I17" s="7">
-        <v>380</v>
-      </c>
-      <c r="J17" s="20"/>
+        <v>400</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
@@ -2226,18 +2230,20 @@
         <v>42671</v>
       </c>
       <c r="F18" s="20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>69</v>
       </c>
       <c r="H18" s="20">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="I18" s="7">
-        <v>1700</v>
-      </c>
-      <c r="J18" s="20"/>
+        <v>1340</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
@@ -2265,7 +2271,9 @@
       <c r="I19" s="7">
         <v>460</v>
       </c>
-      <c r="J19" s="20"/>
+      <c r="J19" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
@@ -2485,15 +2493,15 @@
       <c r="G27" s="20"/>
       <c r="H27" s="20">
         <f>SUBTOTAL(109,Tabela3[Esforço (em horas)])</f>
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="I27" s="7">
         <f>SUM(I3:I26)</f>
-        <v>20570</v>
+        <v>20250</v>
       </c>
       <c r="J27" s="8">
         <f>(COUNTIF(J3:J26,"Concluída")/(COUNTIF(J3:J26,"Concluída") + COUNTIF(J3:J26,"")))</f>
-        <v>0.45833333333333331</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2509,18 +2517,18 @@
       <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
-      <c r="F29" s="26" t="s">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="F29" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
@@ -2538,10 +2546,10 @@
       <c r="F30" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="30"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="22" t="s">
         <v>37</v>
       </c>
@@ -2562,10 +2570,10 @@
       <c r="F31" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="H31" s="25"/>
+      <c r="H31" s="26"/>
       <c r="I31" s="7">
         <v>500</v>
       </c>
@@ -2586,10 +2594,10 @@
       <c r="F32" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="26"/>
       <c r="I32" s="7">
         <v>600</v>
       </c>
@@ -2610,10 +2618,10 @@
       <c r="F33" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="25"/>
+      <c r="H33" s="26"/>
       <c r="I33" s="7">
         <v>2000</v>
       </c>
@@ -2634,10 +2642,10 @@
       <c r="F34" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="24" t="s">
+      <c r="G34" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="H34" s="25"/>
+      <c r="H34" s="26"/>
       <c r="I34" s="7">
         <v>2000</v>
       </c>
@@ -2656,8 +2664,8 @@
         <v>40</v>
       </c>
       <c r="F35" s="21"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="21"/>
     </row>
     <row r="36" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
@@ -2690,6 +2698,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="G34:H34"/>
@@ -2698,7 +2707,6 @@
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="F29:I29"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update CDP and PDC
Atualizado o CDP conforme a execução do projeto e o PDC com a dição de
mais um CDM.
</commit_message>
<xml_diff>
--- a/Projeto/GPR/PG2016-1-CDP.xlsx
+++ b/Projeto/GPR/PG2016-1-CDP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>ID da Atividade</t>
   </si>
@@ -266,9 +266,6 @@
     <t>AT018</t>
   </si>
   <si>
-    <t>AT023</t>
-  </si>
-  <si>
     <t>PG2016-1 – Cronograma do Projeto (CPR)</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>30 dias</t>
+  </si>
+  <si>
+    <t>AT026</t>
   </si>
 </sst>
 </file>
@@ -638,6 +638,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,9 +669,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1715,18 +1715,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="A1" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="24"/>
       <c r="L1" s="23"/>
     </row>
@@ -1986,7 +1986,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="6">
         <v>42654</v>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" s="20">
         <v>2</v>
@@ -2411,7 +2411,7 @@
         <v>2400</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2492,7 +2492,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H26" s="20">
         <v>32</v>
@@ -2501,12 +2501,12 @@
         <v>1600</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="3" t="s">
@@ -2530,14 +2530,16 @@
       <c r="I27" s="7">
         <v>460</v>
       </c>
-      <c r="J27" s="20"/>
+      <c r="J27" s="20" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>34</v>
@@ -2560,7 +2562,9 @@
       <c r="I28" s="7">
         <v>600</v>
       </c>
-      <c r="J28" s="20"/>
+      <c r="J28" s="20" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
@@ -2570,7 +2574,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -2584,7 +2588,7 @@
       </c>
       <c r="J29" s="8">
         <f>(COUNTIF(J3:J28,"Concluída")/(COUNTIF(J3:J28,"Concluída") + COUNTIF(J3:J28,"&lt;&gt;Concluída")))</f>
-        <v>0.69230769230769229</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -2600,18 +2604,18 @@
       <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="F31" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="F31" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
@@ -2627,12 +2631,12 @@
         <v>37</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="32"/>
+      <c r="H32" s="33"/>
       <c r="I32" s="22" t="s">
         <v>37</v>
       </c>
@@ -2651,12 +2655,12 @@
         <v>40</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="26"/>
+        <v>83</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H33" s="27"/>
       <c r="I33" s="7">
         <v>500</v>
       </c>
@@ -2675,12 +2679,12 @@
         <v>44</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="26"/>
+        <v>84</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="H34" s="27"/>
       <c r="I34" s="7">
         <v>600</v>
       </c>
@@ -2699,12 +2703,12 @@
         <v>40</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="H35" s="26"/>
+        <v>85</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="27"/>
       <c r="I35" s="7">
         <v>2000</v>
       </c>
@@ -2723,12 +2727,12 @@
         <v>44</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G36" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="H36" s="26"/>
+        <v>86</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="H36" s="27"/>
       <c r="I36" s="7">
         <v>2000</v>
       </c>
@@ -2747,8 +2751,8 @@
         <v>40</v>
       </c>
       <c r="F37" s="21"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
       <c r="I37" s="21"/>
     </row>
     <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>